<commit_message>
New output S = 20
</commit_message>
<xml_diff>
--- a/Output/DML/Treatment_Effects/DML_BINARY_ESTIMATION_RESULTS.xlsx
+++ b/Output/DML/Treatment_Effects/DML_BINARY_ESTIMATION_RESULTS.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="774" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="830" uniqueCount="101">
   <si>
     <t>outcome</t>
   </si>
@@ -269,6 +269,12 @@
     <t>32.0113890408145 hours</t>
   </si>
   <si>
+    <t>16.4780809044176 hours</t>
+  </si>
+  <si>
+    <t>16.4780811536312 hours</t>
+  </si>
+  <si>
     <t>2023-03-29 16:35:53</t>
   </si>
   <si>
@@ -306,6 +312,9 @@
   </si>
   <si>
     <t>2023-04-03 06:55:58</t>
+  </si>
+  <si>
+    <t>2023-04-04 00:46:31</t>
   </si>
 </sst>
 </file>
@@ -633,7 +642,7 @@
         <v>68</v>
       </c>
       <c r="AT2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3">
@@ -773,7 +782,7 @@
         <v>69</v>
       </c>
       <c r="AT3" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4">
@@ -913,7 +922,7 @@
         <v>69</v>
       </c>
       <c r="AT4" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5">
@@ -1053,7 +1062,7 @@
         <v>69</v>
       </c>
       <c r="AT5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6">
@@ -1193,7 +1202,7 @@
         <v>70</v>
       </c>
       <c r="AT6" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7">
@@ -1333,7 +1342,7 @@
         <v>71</v>
       </c>
       <c r="AT7" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8">
@@ -1473,7 +1482,7 @@
         <v>71</v>
       </c>
       <c r="AT8" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9">
@@ -1613,7 +1622,7 @@
         <v>71</v>
       </c>
       <c r="AT9" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10">
@@ -1753,7 +1762,7 @@
         <v>72</v>
       </c>
       <c r="AT10" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11">
@@ -1893,7 +1902,7 @@
         <v>72</v>
       </c>
       <c r="AT11" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="12">
@@ -2033,7 +2042,7 @@
         <v>72</v>
       </c>
       <c r="AT12" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13">
@@ -2173,7 +2182,7 @@
         <v>72</v>
       </c>
       <c r="AT13" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="14">
@@ -2313,7 +2322,7 @@
         <v>73</v>
       </c>
       <c r="AT14" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15">
@@ -2453,7 +2462,7 @@
         <v>73</v>
       </c>
       <c r="AT15" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16">
@@ -2593,7 +2602,7 @@
         <v>73</v>
       </c>
       <c r="AT16" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="17">
@@ -2733,7 +2742,7 @@
         <v>73</v>
       </c>
       <c r="AT17" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="18">
@@ -2873,7 +2882,7 @@
         <v>74</v>
       </c>
       <c r="AT18" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="19">
@@ -3013,7 +3022,7 @@
         <v>74</v>
       </c>
       <c r="AT19" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="20">
@@ -3153,7 +3162,7 @@
         <v>74</v>
       </c>
       <c r="AT20" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="21">
@@ -3293,7 +3302,7 @@
         <v>74</v>
       </c>
       <c r="AT21" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="22">
@@ -3433,7 +3442,7 @@
         <v>75</v>
       </c>
       <c r="AT22" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="23">
@@ -3573,7 +3582,7 @@
         <v>76</v>
       </c>
       <c r="AT23" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="24">
@@ -3713,7 +3722,7 @@
         <v>76</v>
       </c>
       <c r="AT24" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="25">
@@ -3853,7 +3862,7 @@
         <v>76</v>
       </c>
       <c r="AT25" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="26">
@@ -3993,7 +4002,7 @@
         <v>77</v>
       </c>
       <c r="AT26" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="27">
@@ -4133,7 +4142,7 @@
         <v>78</v>
       </c>
       <c r="AT27" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="28">
@@ -4273,7 +4282,7 @@
         <v>78</v>
       </c>
       <c r="AT28" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="29">
@@ -4413,7 +4422,7 @@
         <v>78</v>
       </c>
       <c r="AT29" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="30">
@@ -4553,7 +4562,7 @@
         <v>79</v>
       </c>
       <c r="AT30" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="31">
@@ -4693,7 +4702,7 @@
         <v>79</v>
       </c>
       <c r="AT31" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="32">
@@ -4833,7 +4842,7 @@
         <v>79</v>
       </c>
       <c r="AT32" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="33">
@@ -4973,7 +4982,7 @@
         <v>79</v>
       </c>
       <c r="AT33" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="34">
@@ -5113,7 +5122,7 @@
         <v>80</v>
       </c>
       <c r="AT34" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="35">
@@ -5253,7 +5262,7 @@
         <v>80</v>
       </c>
       <c r="AT35" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="36">
@@ -5393,7 +5402,7 @@
         <v>80</v>
       </c>
       <c r="AT36" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="37">
@@ -5533,7 +5542,7 @@
         <v>80</v>
       </c>
       <c r="AT37" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="38">
@@ -5673,7 +5682,7 @@
         <v>81</v>
       </c>
       <c r="AT38" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="39">
@@ -5813,7 +5822,7 @@
         <v>81</v>
       </c>
       <c r="AT39" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="40">
@@ -5953,7 +5962,7 @@
         <v>81</v>
       </c>
       <c r="AT40" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="41">
@@ -6093,7 +6102,7 @@
         <v>81</v>
       </c>
       <c r="AT41" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="42">
@@ -6233,7 +6242,7 @@
         <v>82</v>
       </c>
       <c r="AT42" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="43">
@@ -6373,7 +6382,7 @@
         <v>82</v>
       </c>
       <c r="AT43" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="44">
@@ -6513,7 +6522,7 @@
         <v>82</v>
       </c>
       <c r="AT44" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="45">
@@ -6653,7 +6662,7 @@
         <v>82</v>
       </c>
       <c r="AT45" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="46">
@@ -6793,7 +6802,7 @@
         <v>83</v>
       </c>
       <c r="AT46" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="47">
@@ -6933,7 +6942,7 @@
         <v>83</v>
       </c>
       <c r="AT47" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="48">
@@ -7073,7 +7082,7 @@
         <v>83</v>
       </c>
       <c r="AT48" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="49">
@@ -7213,7 +7222,7 @@
         <v>83</v>
       </c>
       <c r="AT49" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="50">
@@ -7353,7 +7362,7 @@
         <v>84</v>
       </c>
       <c r="AT50" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="51">
@@ -7493,7 +7502,7 @@
         <v>84</v>
       </c>
       <c r="AT51" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="52">
@@ -7633,7 +7642,7 @@
         <v>84</v>
       </c>
       <c r="AT52" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="53">
@@ -7773,7 +7782,567 @@
         <v>84</v>
       </c>
       <c r="AT53" t="s">
-        <v>97</v>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s">
+        <v>46</v>
+      </c>
+      <c r="B54" t="s">
+        <v>47</v>
+      </c>
+      <c r="C54" t="s">
+        <v>49</v>
+      </c>
+      <c r="D54" t="s">
+        <v>51</v>
+      </c>
+      <c r="E54" t="s">
+        <v>53</v>
+      </c>
+      <c r="F54" t="s">
+        <v>52</v>
+      </c>
+      <c r="G54" t="s">
+        <v>54</v>
+      </c>
+      <c r="H54" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="I54" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="J54" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="K54" t="s">
+        <v>58</v>
+      </c>
+      <c r="L54" t="s">
+        <v>62</v>
+      </c>
+      <c r="M54" t="s">
+        <v>53</v>
+      </c>
+      <c r="N54" t="n">
+        <v>11122.0</v>
+      </c>
+      <c r="O54" t="n">
+        <v>11117.0</v>
+      </c>
+      <c r="P54" t="n">
+        <v>29.3275</v>
+      </c>
+      <c r="Q54" t="n">
+        <v>81.3</v>
+      </c>
+      <c r="R54" t="n">
+        <v>50.46</v>
+      </c>
+      <c r="S54" t="s">
+        <v>50</v>
+      </c>
+      <c r="T54" t="s">
+        <v>64</v>
+      </c>
+      <c r="U54" t="n">
+        <v>0.006448414444749802</v>
+      </c>
+      <c r="V54" t="n">
+        <v>0.0063458116204920915</v>
+      </c>
+      <c r="W54" t="n">
+        <v>0.00586027410042029</v>
+      </c>
+      <c r="X54" t="n">
+        <v>0.004210494688011051</v>
+      </c>
+      <c r="Y54" t="n">
+        <v>1.1432440603525185</v>
+      </c>
+      <c r="Z54" t="n">
+        <v>1.5285777332213555</v>
+      </c>
+      <c r="AA54" t="n">
+        <v>0.27229161339660796</v>
+      </c>
+      <c r="AB54" t="n">
+        <v>0.1263975975859819</v>
+      </c>
+      <c r="AC54" t="n">
+        <v>0.006430679805759445</v>
+      </c>
+      <c r="AD54" t="n">
+        <v>0.006466149083740158</v>
+      </c>
+      <c r="AE54" t="n">
+        <v>0.006333069622083291</v>
+      </c>
+      <c r="AF54" t="n">
+        <v>0.006358553618900892</v>
+      </c>
+      <c r="AG54" t="n">
+        <v>0.8187340963852295</v>
+      </c>
+      <c r="AH54" t="n">
+        <v>0.18039209516533683</v>
+      </c>
+      <c r="AI54" t="n">
+        <v>0.5636796091397615</v>
+      </c>
+      <c r="AJ54" t="n">
+        <v>0.7394059918206516</v>
+      </c>
+      <c r="AK54" t="n">
+        <v>0.4907011215366788</v>
+      </c>
+      <c r="AL54" t="n">
+        <v>0.5181675881025801</v>
+      </c>
+      <c r="AM54" t="n">
+        <v>251.09413390640668</v>
+      </c>
+      <c r="AN54" t="n">
+        <v>269.898349306286</v>
+      </c>
+      <c r="AO54" t="n">
+        <v>0.41150056245865535</v>
+      </c>
+      <c r="AP54" t="n">
+        <v>0.45090114000864906</v>
+      </c>
+      <c r="AQ54" t="n">
+        <v>0.6413301610949432</v>
+      </c>
+      <c r="AR54" t="n">
+        <v>0.670904004914734</v>
+      </c>
+      <c r="AS54" t="s">
+        <v>85</v>
+      </c>
+      <c r="AT54" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s">
+        <v>46</v>
+      </c>
+      <c r="B55" t="s">
+        <v>47</v>
+      </c>
+      <c r="C55" t="s">
+        <v>49</v>
+      </c>
+      <c r="D55" t="s">
+        <v>51</v>
+      </c>
+      <c r="E55" t="s">
+        <v>53</v>
+      </c>
+      <c r="F55" t="s">
+        <v>52</v>
+      </c>
+      <c r="G55" t="s">
+        <v>54</v>
+      </c>
+      <c r="H55" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="I55" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="J55" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="K55" t="s">
+        <v>58</v>
+      </c>
+      <c r="L55" t="s">
+        <v>62</v>
+      </c>
+      <c r="M55" t="s">
+        <v>53</v>
+      </c>
+      <c r="N55" t="n">
+        <v>11122.0</v>
+      </c>
+      <c r="O55" t="n">
+        <v>11117.0</v>
+      </c>
+      <c r="P55" t="n">
+        <v>29.3275</v>
+      </c>
+      <c r="Q55" t="n">
+        <v>81.3</v>
+      </c>
+      <c r="R55" t="n">
+        <v>50.46</v>
+      </c>
+      <c r="S55" t="s">
+        <v>63</v>
+      </c>
+      <c r="T55" t="s">
+        <v>65</v>
+      </c>
+      <c r="U55" t="n">
+        <v>-0.03250071298585326</v>
+      </c>
+      <c r="V55" t="n">
+        <v>-0.033667872232583475</v>
+      </c>
+      <c r="W55" t="n">
+        <v>0.016275683729889523</v>
+      </c>
+      <c r="X55" t="n">
+        <v>0.016208876818408095</v>
+      </c>
+      <c r="Y55" t="n">
+        <v>-1.9972308491074615</v>
+      </c>
+      <c r="Z55" t="n">
+        <v>-2.061890683621395</v>
+      </c>
+      <c r="AA55" t="n">
+        <v>0.04714637619472564</v>
+      </c>
+      <c r="AB55" t="n">
+        <v>0.039241323127657796</v>
+      </c>
+      <c r="AC55" t="n">
+        <v>-0.03254996723067606</v>
+      </c>
+      <c r="AD55" t="n">
+        <v>-0.03245145874103046</v>
+      </c>
+      <c r="AE55" t="n">
+        <v>-0.033716924303167174</v>
+      </c>
+      <c r="AF55" t="n">
+        <v>-0.033618820161999775</v>
+      </c>
+      <c r="AG55" t="n">
+        <v>0.8187340963852295</v>
+      </c>
+      <c r="AH55" t="n">
+        <v>0.18039209516533683</v>
+      </c>
+      <c r="AI55" t="n">
+        <v>0.5636796091397615</v>
+      </c>
+      <c r="AJ55" t="n">
+        <v>0.7394059918206516</v>
+      </c>
+      <c r="AK55" t="n">
+        <v>0.4907011215366788</v>
+      </c>
+      <c r="AL55" t="n">
+        <v>0.5181675881025801</v>
+      </c>
+      <c r="AM55" t="n">
+        <v>251.09413390640668</v>
+      </c>
+      <c r="AN55" t="n">
+        <v>269.898349306286</v>
+      </c>
+      <c r="AO55" t="n">
+        <v>0.41150056245865535</v>
+      </c>
+      <c r="AP55" t="n">
+        <v>0.45090114000864906</v>
+      </c>
+      <c r="AQ55" t="n">
+        <v>0.6413301610949432</v>
+      </c>
+      <c r="AR55" t="n">
+        <v>0.670904004914734</v>
+      </c>
+      <c r="AS55" t="s">
+        <v>86</v>
+      </c>
+      <c r="AT55" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s">
+        <v>46</v>
+      </c>
+      <c r="B56" t="s">
+        <v>47</v>
+      </c>
+      <c r="C56" t="s">
+        <v>49</v>
+      </c>
+      <c r="D56" t="s">
+        <v>51</v>
+      </c>
+      <c r="E56" t="s">
+        <v>53</v>
+      </c>
+      <c r="F56" t="s">
+        <v>52</v>
+      </c>
+      <c r="G56" t="s">
+        <v>54</v>
+      </c>
+      <c r="H56" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="I56" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="J56" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="K56" t="s">
+        <v>58</v>
+      </c>
+      <c r="L56" t="s">
+        <v>62</v>
+      </c>
+      <c r="M56" t="s">
+        <v>53</v>
+      </c>
+      <c r="N56" t="n">
+        <v>11122.0</v>
+      </c>
+      <c r="O56" t="n">
+        <v>11117.0</v>
+      </c>
+      <c r="P56" t="n">
+        <v>29.3275</v>
+      </c>
+      <c r="Q56" t="n">
+        <v>81.3</v>
+      </c>
+      <c r="R56" t="n">
+        <v>50.46</v>
+      </c>
+      <c r="S56" t="s">
+        <v>63</v>
+      </c>
+      <c r="T56" t="s">
+        <v>66</v>
+      </c>
+      <c r="U56" t="n">
+        <v>-0.03172562267050359</v>
+      </c>
+      <c r="V56" t="n">
+        <v>-0.031737564722237696</v>
+      </c>
+      <c r="W56" t="n">
+        <v>0.01379196527947356</v>
+      </c>
+      <c r="X56" t="n">
+        <v>0.013800067207272749</v>
+      </c>
+      <c r="Y56" t="n">
+        <v>-2.3003119953999787</v>
+      </c>
+      <c r="Z56" t="n">
+        <v>-2.305891994179437</v>
+      </c>
+      <c r="AA56" t="n">
+        <v>0.022750711970795257</v>
+      </c>
+      <c r="AB56" t="n">
+        <v>0.02113497066269257</v>
+      </c>
+      <c r="AC56" t="n">
+        <v>-0.031767360568937635</v>
+      </c>
+      <c r="AD56" t="n">
+        <v>-0.03168388477206955</v>
+      </c>
+      <c r="AE56" t="n">
+        <v>-0.031779327139109304</v>
+      </c>
+      <c r="AF56" t="n">
+        <v>-0.03169580230536609</v>
+      </c>
+      <c r="AG56" t="n">
+        <v>0.8187340963852295</v>
+      </c>
+      <c r="AH56" t="n">
+        <v>0.18039209516533683</v>
+      </c>
+      <c r="AI56" t="n">
+        <v>0.5636796091397615</v>
+      </c>
+      <c r="AJ56" t="n">
+        <v>0.7394059918206516</v>
+      </c>
+      <c r="AK56" t="n">
+        <v>0.4907011215366788</v>
+      </c>
+      <c r="AL56" t="n">
+        <v>0.5181675881025801</v>
+      </c>
+      <c r="AM56" t="n">
+        <v>251.09413390640668</v>
+      </c>
+      <c r="AN56" t="n">
+        <v>269.898349306286</v>
+      </c>
+      <c r="AO56" t="n">
+        <v>0.41150056245865535</v>
+      </c>
+      <c r="AP56" t="n">
+        <v>0.45090114000864906</v>
+      </c>
+      <c r="AQ56" t="n">
+        <v>0.6413301610949432</v>
+      </c>
+      <c r="AR56" t="n">
+        <v>0.670904004914734</v>
+      </c>
+      <c r="AS56" t="s">
+        <v>86</v>
+      </c>
+      <c r="AT56" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s">
+        <v>46</v>
+      </c>
+      <c r="B57" t="s">
+        <v>47</v>
+      </c>
+      <c r="C57" t="s">
+        <v>49</v>
+      </c>
+      <c r="D57" t="s">
+        <v>51</v>
+      </c>
+      <c r="E57" t="s">
+        <v>53</v>
+      </c>
+      <c r="F57" t="s">
+        <v>52</v>
+      </c>
+      <c r="G57" t="s">
+        <v>54</v>
+      </c>
+      <c r="H57" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="I57" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="J57" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="K57" t="s">
+        <v>58</v>
+      </c>
+      <c r="L57" t="s">
+        <v>62</v>
+      </c>
+      <c r="M57" t="s">
+        <v>53</v>
+      </c>
+      <c r="N57" t="n">
+        <v>11122.0</v>
+      </c>
+      <c r="O57" t="n">
+        <v>11117.0</v>
+      </c>
+      <c r="P57" t="n">
+        <v>29.3275</v>
+      </c>
+      <c r="Q57" t="n">
+        <v>81.3</v>
+      </c>
+      <c r="R57" t="n">
+        <v>50.46</v>
+      </c>
+      <c r="S57" t="s">
+        <v>53</v>
+      </c>
+      <c r="T57" t="s">
+        <v>67</v>
+      </c>
+      <c r="U57" t="n">
+        <v>-0.02605229854110346</v>
+      </c>
+      <c r="V57" t="n">
+        <v>-0.0265058312944634</v>
+      </c>
+      <c r="W57" t="n">
+        <v>0.007956742527413576</v>
+      </c>
+      <c r="X57" t="n">
+        <v>0.005445171150942421</v>
+      </c>
+      <c r="Y57" t="n">
+        <v>-3.3500071697880087</v>
+      </c>
+      <c r="Z57" t="n">
+        <v>-4.5560050377228425</v>
+      </c>
+      <c r="AA57" t="n">
+        <v>0.0019845663800074297</v>
+      </c>
+      <c r="AB57" t="n">
+        <v>5.269068479047221E-6</v>
+      </c>
+      <c r="AC57" t="n">
+        <v>-0.026076377612123836</v>
+      </c>
+      <c r="AD57" t="n">
+        <v>-0.026028219470083082</v>
+      </c>
+      <c r="AE57" t="n">
+        <v>-0.026522309729251244</v>
+      </c>
+      <c r="AF57" t="n">
+        <v>-0.026489352859675554</v>
+      </c>
+      <c r="AG57" t="n">
+        <v>0.8187340963852295</v>
+      </c>
+      <c r="AH57" t="n">
+        <v>0.18039209516533683</v>
+      </c>
+      <c r="AI57" t="n">
+        <v>0.5636796091397615</v>
+      </c>
+      <c r="AJ57" t="n">
+        <v>0.7394059918206516</v>
+      </c>
+      <c r="AK57" t="n">
+        <v>0.4907011215366788</v>
+      </c>
+      <c r="AL57" t="n">
+        <v>0.5181675881025801</v>
+      </c>
+      <c r="AM57" t="n">
+        <v>251.09413390640668</v>
+      </c>
+      <c r="AN57" t="n">
+        <v>269.898349306286</v>
+      </c>
+      <c r="AO57" t="n">
+        <v>0.41150056245865535</v>
+      </c>
+      <c r="AP57" t="n">
+        <v>0.45090114000864906</v>
+      </c>
+      <c r="AQ57" t="n">
+        <v>0.6413301610949432</v>
+      </c>
+      <c r="AR57" t="n">
+        <v>0.670904004914734</v>
+      </c>
+      <c r="AS57" t="s">
+        <v>86</v>
+      </c>
+      <c r="AT57" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>